<commit_message>
Seperated HD Non OOP into seperate functions
</commit_message>
<xml_diff>
--- a/data_files/Appliance-Pricing-10-1-18.xlsx
+++ b/data_files/Appliance-Pricing-10-1-18.xlsx
@@ -295,621 +295,592 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>409</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>409</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>409</v>
+      <c r="H2" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>26</v>
+      <c r="K2" s="0" t="n">
+        <v>599</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>599</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>599</v>
+      <c r="N2" s="0" t="n">
+        <v>19.835</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>19.835</v>
+        <v>145</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>145</v>
+        <v>883049415956</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>883049415956</v>
+        <v>43.75</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>43.75</v>
+        <v>27.25</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>27.25</v>
-      </c>
-      <c r="T2" s="0" t="n">
         <v>28.75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>409</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>409</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>409</v>
+      <c r="H3" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>26</v>
+      <c r="K3" s="0" t="n">
+        <v>599</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>599</v>
       </c>
-      <c r="M3" s="0" t="n">
-        <v>599</v>
+      <c r="N3" s="0" t="n">
+        <v>19.835</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>19.835</v>
+        <v>145</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>145</v>
+        <v>883049415956</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>883049415956</v>
+        <v>43.75</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>43.75</v>
+        <v>27.25</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>27.25</v>
-      </c>
-      <c r="T3" s="0" t="n">
         <v>28.75</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="V3" s="0" t="n">
         <v>398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>30</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>409</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>409</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>409</v>
+      <c r="H4" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>26</v>
+      <c r="K4" s="0" t="n">
+        <v>599</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>599</v>
       </c>
-      <c r="M4" s="0" t="n">
-        <v>599</v>
+      <c r="N4" s="0" t="n">
+        <v>22.491</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>22.491</v>
+        <v>117</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>117</v>
+        <v>883049348339</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>883049348339</v>
+        <v>43.5</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>43.5</v>
+        <v>29.13</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="T4" s="0" t="n">
         <v>30.67</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="V4" s="0" t="n">
         <v>398</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>33</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>489</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>489</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>489</v>
+      <c r="H6" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>26</v>
+      <c r="K6" s="0" t="n">
+        <v>699</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>699</v>
       </c>
-      <c r="M6" s="0" t="n">
-        <v>699</v>
+      <c r="N6" s="0" t="n">
+        <v>22.491</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>22.491</v>
+        <v>124</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>124</v>
+        <v>883049348599</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>883049348599</v>
+        <v>43.5</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>43.5</v>
+        <v>29.13</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="T6" s="0" t="n">
         <v>30.67</v>
       </c>
-      <c r="W6" s="0" t="n">
+      <c r="V6" s="0" t="n">
         <v>498</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>428</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>428</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>428</v>
+      <c r="H7" s="0" t="n">
+        <v>549</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>549</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <v>549</v>
+      <c r="K7" s="0" t="n">
+        <v>649</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>649</v>
       </c>
-      <c r="M7" s="0" t="n">
-        <v>649</v>
+      <c r="N7" s="0" t="n">
+        <v>20.844</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>20.844</v>
+        <v>172</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>172</v>
+        <v>883049408354</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>883049408354</v>
+        <v>46</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="T7" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="W7" s="0" t="s">
+      <c r="V7" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>428</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>428</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>428</v>
+      <c r="H8" s="0" t="n">
+        <v>549</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>549</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <v>549</v>
+      <c r="K8" s="0" t="n">
+        <v>649</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>649</v>
       </c>
-      <c r="M8" s="0" t="n">
-        <v>649</v>
+      <c r="N8" s="0" t="n">
+        <v>22.491</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>22.491</v>
+        <v>124</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>124</v>
+        <v>883049410401</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>883049410401</v>
+        <v>43.5</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>43.5</v>
+        <v>29.13</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="T8" s="0" t="n">
         <v>30.67</v>
       </c>
+      <c r="T8" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="U8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="W8" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>508</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>508</v>
+      <c r="H9" s="0" t="n">
+        <v>649</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>649</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>649</v>
+      <c r="K9" s="0" t="n">
+        <v>749</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>749</v>
       </c>
-      <c r="M9" s="0" t="n">
-        <v>749</v>
+      <c r="N9" s="0" t="n">
+        <v>22.491</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>22.491</v>
+        <v>124</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>124</v>
+        <v>883049410425</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>883049410425</v>
+        <v>43.5</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>43.5</v>
+        <v>29.13</v>
       </c>
       <c r="S9" s="0" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="T9" s="0" t="n">
         <v>30.67</v>
       </c>
+      <c r="T9" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="U9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="W9" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="0" t="s">
         <v>45</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>566</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>566</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>566</v>
+      <c r="H10" s="0" t="n">
+        <v>699</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>699</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>699</v>
+      <c r="K10" s="0" t="n">
+        <v>799</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>799</v>
       </c>
-      <c r="M10" s="0" t="n">
-        <v>799</v>
+      <c r="N10" s="0" t="n">
+        <v>21.124</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>21.124</v>
+        <v>120</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>120</v>
+        <v>883049392240</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>883049392240</v>
+        <v>43.5</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>43.5</v>
+        <v>27.36</v>
       </c>
       <c r="S10" s="0" t="n">
-        <v>27.36</v>
-      </c>
-      <c r="T10" s="0" t="n">
         <v>30.67</v>
       </c>
+      <c r="T10" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="U10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="W10" s="0" t="n">
+      <c r="V10" s="0" t="n">
         <v>639</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="0" t="s">
         <v>48</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>646</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>646</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>646</v>
+      <c r="H11" s="0" t="n">
+        <v>799</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>799</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <v>799</v>
+      <c r="K11" s="0" t="n">
+        <v>899</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>899</v>
       </c>
-      <c r="M11" s="0" t="n">
-        <v>899</v>
+      <c r="N11" s="0" t="n">
+        <v>21.124</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>21.124</v>
+        <v>124</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>124</v>
+        <v>883049392257</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>883049392257</v>
+        <v>43.5</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>43.5</v>
+        <v>27.36</v>
       </c>
       <c r="S11" s="0" t="n">
-        <v>27.36</v>
-      </c>
-      <c r="T11" s="0" t="n">
         <v>30.67</v>
       </c>
+      <c r="T11" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="U11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="V11" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="W11" s="0" t="n">
+      <c r="V11" s="0" t="n">
         <v>719</v>
       </c>
     </row>

</xml_diff>